<commit_message>
app will choose correct overlay depending on mobile vs desktop
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -399,7 +399,7 @@
         <v>edarko@darko.com</v>
       </c>
       <c r="C2" t="str">
-        <v>http://08c535d5720f9753c0e1-b8d20a8cf0fc9d80e5b0d6e172309654.r56.cf1.rackcdn.com/webpages-1596592697021</v>
+        <v>http://08c535d5720f9753c0e1-b8d20a8cf0fc9d80e5b0d6e172309654.r56.cf1.rackcdn.com/webpages-1596682944123</v>
       </c>
     </row>
     <row r="3">
@@ -410,7 +410,7 @@
         <v>pdora@pandora.com</v>
       </c>
       <c r="C3" t="str">
-        <v>http://08c535d5720f9753c0e1-b8d20a8cf0fc9d80e5b0d6e172309654.r56.cf1.rackcdn.com/webpages-1596592702768</v>
+        <v>http://08c535d5720f9753c0e1-b8d20a8cf0fc9d80e5b0d6e172309654.r56.cf1.rackcdn.com/webpages-1596682948750</v>
       </c>
     </row>
     <row r="4">
@@ -421,7 +421,7 @@
         <v>pwurple@pwerp.com</v>
       </c>
       <c r="C4" t="str">
-        <v>http://08c535d5720f9753c0e1-b8d20a8cf0fc9d80e5b0d6e172309654.r56.cf1.rackcdn.com/webpages-1596592710199</v>
+        <v>http://08c535d5720f9753c0e1-b8d20a8cf0fc9d80e5b0d6e172309654.r56.cf1.rackcdn.com/webpages-1596682954194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>